<commit_message>
add pdf of top ind
</commit_message>
<xml_diff>
--- a/pendulum/part_obs_pendulum/excel_sheets/part_obs_training_data.xlsx
+++ b/pendulum/part_obs_pendulum/excel_sheets/part_obs_training_data.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -472,6 +472,546 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>-1079.124164279027</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-848.469530548085</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-848.469530548085</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-843.0308251850365</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-422.9664883515331</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-422.9664883515331</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-422.9664883515331</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-422.9664883515331</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-422.9664883515331</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-408.1464943031704</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-418.1918056887311</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-391.8626217612404</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-391.8626217612404</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-391.8626217612404</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-359.0143706184192</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-391.8626217612404</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-391.8626217612404</v>
+      </c>
+      <c r="R3" t="n">
+        <v>-391.8626217612404</v>
+      </c>
+      <c r="S3" t="n">
+        <v>-378.0698146577363</v>
+      </c>
+      <c r="T3" t="n">
+        <v>-368.8161587816912</v>
+      </c>
+      <c r="U3" t="n">
+        <v>-368.8161587816912</v>
+      </c>
+      <c r="V3" t="n">
+        <v>-368.8161587816912</v>
+      </c>
+      <c r="W3" t="n">
+        <v>-297.3756495472674</v>
+      </c>
+      <c r="X3" t="n">
+        <v>-295.9146378649457</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>-295.9146378649457</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>-276.3300181151498</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>-276</v>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>protectedDiv(ang_vel(ang_vel(sin(add(x1, x3)), sin(y1), protectedDiv(y2, y2), acos(y3, y1)), y3, sub(sin(x2), sin(x1)), x2), acos(limit(add(y3, y1), tan(y3), limit(y3, limit(x1, conditional(max(limit(x1, y2, y2), asin(x2, x2)), protectedDiv(y3, y1)), y2), x3)), y3))</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">atan, cos, </t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">asin, sub, y2, ang_vel, y3, conditional, add, x1, acos, x2, limit, x3, tan, protectedDiv, sin, max, y1, </t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>replace</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-1442.308611964176</v>
+      </c>
+      <c r="B4" t="n">
+        <v>-1442.308611964176</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-1210.076479151252</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-1122.265024527062</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-922.6883893958251</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-917.517353073861</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-888.5983683439032</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-881.8947934595822</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-888.5983683439032</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-842.7434668940824</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-842.7434668940824</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-818.2019360255579</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-805.8377446780125</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-805.8377446780125</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-805.8377446780125</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-805.8377446780125</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-805.8377446780125</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-805.8377446780125</v>
+      </c>
+      <c r="S4" t="n">
+        <v>-805.8377446780125</v>
+      </c>
+      <c r="T4" t="n">
+        <v>-805.8377446780125</v>
+      </c>
+      <c r="U4" t="n">
+        <v>-805.8377446780125</v>
+      </c>
+      <c r="V4" t="n">
+        <v>-805.8377446780125</v>
+      </c>
+      <c r="W4" t="n">
+        <v>-805.8377446780125</v>
+      </c>
+      <c r="X4" t="n">
+        <v>-805.8377446780125</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>-805.8377446780125</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>-798.8856563967825</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>-798</v>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>sub(max(cos(x1), max(cos(y3), max(cos(y3), x3))), ang_vel(y1, y2, y2, x2))</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">asin, conditional, add, atan, acos, limit, tan, protectedDiv, sin, </t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">sub, y2, y3, ang_vel, x1, x2, cos, x3, max, y1, </t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>replace</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>-1619.964498509805</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-1619.964498509805</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-1299.238280821162</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-1299.238280821162</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1299.238280821162</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-1299.238280821162</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-1082.216647383359</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-1151.103452580407</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-1091.628168703129</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-1091.628168703129</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-986.9940741711816</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-983.3046702951158</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-974.2705400266841</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-974.2705400266841</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-913.2553578182371</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-913.2553578182371</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-913.2553578182371</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-752.0061341960293</v>
+      </c>
+      <c r="S5" t="n">
+        <v>-752.0061341960293</v>
+      </c>
+      <c r="T5" t="n">
+        <v>-732.7577570647497</v>
+      </c>
+      <c r="U5" t="n">
+        <v>-617.5256876666257</v>
+      </c>
+      <c r="V5" t="n">
+        <v>-607.8416502439702</v>
+      </c>
+      <c r="W5" t="n">
+        <v>-607.8416502439702</v>
+      </c>
+      <c r="X5" t="n">
+        <v>-607.8416502439702</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>-607.8416502439702</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>-607.8416502439702</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>-607</v>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>atan(conditional(x3, x1), protectedDiv(conditional(atan(x2, x1), y2), ang_vel(y1, y2, x3, max(conditional(add(y2, x3), conditional(sub(y3, y3), y2)), cos(x1)))))</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">asin, acos, limit, tan, sin, </t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">sub, y2, ang_vel, conditional, y3, atan, x1, add, protectedDiv, x2, cos, x3, max, y1, </t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>replace</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>-1941.031432860915</v>
+      </c>
+      <c r="B6" t="n">
+        <v>-1791.499395120618</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-1370.454336709915</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-1370.454336709915</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-1370.454336709915</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-1370.454336709915</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-829.7111171653264</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-829.7111171653264</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-749.728351271869</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-520.2006354645862</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-581.6375869088503</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-507.9621848295731</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-424.7650624491251</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-405.5134734374636</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-372.5741659638643</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-372.5741659638643</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-350.6699524222988</v>
+      </c>
+      <c r="R6" t="n">
+        <v>-350.6699524222988</v>
+      </c>
+      <c r="S6" t="n">
+        <v>-350.6699524222988</v>
+      </c>
+      <c r="T6" t="n">
+        <v>-310.4468697023653</v>
+      </c>
+      <c r="U6" t="n">
+        <v>-310.4468697023653</v>
+      </c>
+      <c r="V6" t="n">
+        <v>-280.1756378190058</v>
+      </c>
+      <c r="W6" t="n">
+        <v>-280.1756378190058</v>
+      </c>
+      <c r="X6" t="n">
+        <v>-280.1756378190058</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>-254.2868649148867</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>-280.1756378190058</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>-254</v>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>sub(ang_vel(conditional(x2, sub(asin(asin(y2, x1), y1), y1)), tan(protectedDiv(x1, y1)), sin(x2), conditional(y2, limit(x1, y2, sub(atan(x1, x3), acos(y3, x1))))), y1)</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">add, cos, max, </t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">asin, sub, y2, ang_vel, conditional, y3, x1, atan, acos, x2, limit, x3, tan, protectedDiv, sin, y1, </t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>replace</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-1731.721096382269</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-1417.990154509263</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-1680.526693179986</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-1121.590165741666</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-1121.590165741666</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-1076.506884726996</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-1076.506884726996</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-942.081698275406</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-978.3045941305334</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-870.1673564621833</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-870.1673564621833</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-870.1673564621833</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-870.1673564621833</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-434.047639160293</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-434.047639160293</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-394.9991729263456</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-394.9991729263456</v>
+      </c>
+      <c r="R7" t="n">
+        <v>-394.9991729263456</v>
+      </c>
+      <c r="S7" t="n">
+        <v>-424.1300170352418</v>
+      </c>
+      <c r="T7" t="n">
+        <v>-291.123804233541</v>
+      </c>
+      <c r="U7" t="n">
+        <v>-291.123804233541</v>
+      </c>
+      <c r="V7" t="n">
+        <v>-291.123804233541</v>
+      </c>
+      <c r="W7" t="n">
+        <v>-291.123804233541</v>
+      </c>
+      <c r="X7" t="n">
+        <v>-291.123804233541</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>-291.123804233541</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>-291.123804233541</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>-291</v>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>atan(acos(limit(y2, x1, x3), tan(y2)), sub(x3, atan(x3, y1)))</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">asin, ang_vel, conditional, y3, add, x2, cos, protectedDiv, sin, max, </t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">sub, y2, x1, atan, acos, limit, tan, x3, y1, </t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>replace</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Create tree pdf of best ind
</commit_message>
<xml_diff>
--- a/pendulum/part_obs_pendulum/excel_sheets/part_obs_training_data.xlsx
+++ b/pendulum/part_obs_pendulum/excel_sheets/part_obs_training_data.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF7"/>
+  <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1012,6 +1012,546 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>-1450.392252482472</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-1450.392252482472</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-1450.392252482472</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-1339.250701011006</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-1339.250701011006</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-1034.248189140555</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-1247.897379399485</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-1225.78532072732</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-971.5862553205345</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-845.5579614850009</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-845.5579614850009</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-822.3941131771093</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-822.3941131771093</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-809.1449917242714</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-809.1449917242714</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-809.1449917242714</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-774.5200934940744</v>
+      </c>
+      <c r="R8" t="n">
+        <v>-774.5200934940744</v>
+      </c>
+      <c r="S8" t="n">
+        <v>-774.5200934940744</v>
+      </c>
+      <c r="T8" t="n">
+        <v>-774.5200934940744</v>
+      </c>
+      <c r="U8" t="n">
+        <v>-606.1629503574208</v>
+      </c>
+      <c r="V8" t="n">
+        <v>-606.1629503574208</v>
+      </c>
+      <c r="W8" t="n">
+        <v>-606.1629503574208</v>
+      </c>
+      <c r="X8" t="n">
+        <v>-606.1629503574208</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>-606.1629503574208</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>-606.1629503574208</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>-606</v>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>sub(protectedDiv(add(protectedDiv(add(x3, y3), y2), conditional(y2, y1)), y3), tan(ang_vel(x3, y1, y3, x1)))</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">max, atan, limit, acos, x2, cos, asin, sin, </t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tan, y2, ang_vel, sub, protectedDiv, conditional, y1, x1, y3, x3, add, </t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>replace</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>-1846.511939803875</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-1814.824988986811</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-1643.775424731376</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-1578.434304670724</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-1611.060645760238</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-1571.749795489733</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-1562.356788893979</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-1514.481553625497</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-1471.719288795401</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-839.9296345291842</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-555.7937755520754</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-555.7937755520754</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-555.7937755520754</v>
+      </c>
+      <c r="N9" t="n">
+        <v>-491.9180312454844</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-491.9180312454844</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-368.582643133616</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-491.9180312454844</v>
+      </c>
+      <c r="R9" t="n">
+        <v>-470.7954276157421</v>
+      </c>
+      <c r="S9" t="n">
+        <v>-422.3190395215176</v>
+      </c>
+      <c r="T9" t="n">
+        <v>-390.5510587169434</v>
+      </c>
+      <c r="U9" t="n">
+        <v>-390.5510587169434</v>
+      </c>
+      <c r="V9" t="n">
+        <v>-390.5510587169434</v>
+      </c>
+      <c r="W9" t="n">
+        <v>-386.6780925103196</v>
+      </c>
+      <c r="X9" t="n">
+        <v>-339.7634857551262</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>-339.7634857551262</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>-339.7634857551262</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>-339</v>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>ang_vel(add(atan(protectedDiv(limit(x1, x1, x1), cos(y3)), y1), acos(y3, x2)), tan(ang_vel(x1, x1, y1, x2)), tan(atan(x2, x3)), sub(y3, atan(limit(x1, y2, x3), y1)))</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">max, conditional, asin, sin, </t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tan, ang_vel, y2, atan, protectedDiv, limit, y1, acos, x2, sub, x1, y3, x3, add, cos, </t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>replace</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>-1789.86075472485</v>
+      </c>
+      <c r="B10" t="n">
+        <v>-1528.037694102767</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-1528.037694102767</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-1357.045211674417</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-1357.045211674417</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-1161.658315096036</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-1161.658315096036</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-1161.658315096036</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-1153.448653591956</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-1136.089205368618</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-1136.089205368618</v>
+      </c>
+      <c r="L10" t="n">
+        <v>-1136.089205368618</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-1120.588294685263</v>
+      </c>
+      <c r="N10" t="n">
+        <v>-1120.588294685263</v>
+      </c>
+      <c r="O10" t="n">
+        <v>-1097.867324816126</v>
+      </c>
+      <c r="P10" t="n">
+        <v>-1071.788871636817</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-1066.342320838975</v>
+      </c>
+      <c r="R10" t="n">
+        <v>-1040.95524327635</v>
+      </c>
+      <c r="S10" t="n">
+        <v>-1005.576138894399</v>
+      </c>
+      <c r="T10" t="n">
+        <v>-1005.576138894399</v>
+      </c>
+      <c r="U10" t="n">
+        <v>-1005.576138894399</v>
+      </c>
+      <c r="V10" t="n">
+        <v>-984.7614892657341</v>
+      </c>
+      <c r="W10" t="n">
+        <v>-984.7614892657341</v>
+      </c>
+      <c r="X10" t="n">
+        <v>-984.7614892657341</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>-984.7614892657341</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>-984.7614892657341</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>-984</v>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>limit(add(ang_vel(x3, x2, x3, y1), sub(ang_vel(conditional(y3, x3), limit(x2, y3, y2), sub(y3, x3), ang_vel(y2, x2, x1, x1)), y1)), sin(conditional(sin(sin(y2)), y2)), conditional(protectedDiv(limit(x2, y3, y3), x3), sub(y2, y1)))</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">max, tan, atan, acos, cos, asin, </t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ang_vel, y2, limit, sub, y1, conditional, x2, protectedDiv, x1, y3, x3, add, sin, </t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>replace</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>-1869.666379095403</v>
+      </c>
+      <c r="B11" t="n">
+        <v>-1858.017431513293</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-1683.847603090057</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-1638.039076445267</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-1638.039076445267</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-1638.039076445267</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-1561.561743484393</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-1503.110190170663</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-1434.012662221568</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-1441.600235894704</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-1416.57105079192</v>
+      </c>
+      <c r="L11" t="n">
+        <v>-1403.018450573949</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-1363.708964168934</v>
+      </c>
+      <c r="N11" t="n">
+        <v>-1265.797229648083</v>
+      </c>
+      <c r="O11" t="n">
+        <v>-1265.797229648083</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-1265.797229648083</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>-1224.686774815917</v>
+      </c>
+      <c r="R11" t="n">
+        <v>-1224.686774815917</v>
+      </c>
+      <c r="S11" t="n">
+        <v>-1224.686774815917</v>
+      </c>
+      <c r="T11" t="n">
+        <v>-1224.686774815917</v>
+      </c>
+      <c r="U11" t="n">
+        <v>-1224.686774815917</v>
+      </c>
+      <c r="V11" t="n">
+        <v>-1224.686774815917</v>
+      </c>
+      <c r="W11" t="n">
+        <v>-1224.686774815917</v>
+      </c>
+      <c r="X11" t="n">
+        <v>-1115.965253686046</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>-1196.46924446723</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>-1221.312058234421</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>-1115</v>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>limit(atan(acos(x1, asin(x3, y1)), x2), asin(x2, x3), limit(x1, x2, limit(x1, x2, tan(sub(sub(tan(x1), max(y2, y3)), x3)))))</t>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ang_vel, protectedDiv, conditional, add, cos, sin, </t>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">max, tan, y2, limit, atan, y1, sub, acos, x2, x1, y3, x3, asin, </t>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>replace</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>-1734.229883634241</v>
+      </c>
+      <c r="B12" t="n">
+        <v>-1606.824069959779</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-863.7435572017827</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-844.8124702330682</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-747.8722419058496</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-747.8722419058496</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-747.8722419058496</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-747.8722419058496</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-657.8122769901919</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-657.8122769901919</v>
+      </c>
+      <c r="K12" t="n">
+        <v>-633.5609828241129</v>
+      </c>
+      <c r="L12" t="n">
+        <v>-633.5609828241129</v>
+      </c>
+      <c r="M12" t="n">
+        <v>-633.214810131536</v>
+      </c>
+      <c r="N12" t="n">
+        <v>-548.7929538670101</v>
+      </c>
+      <c r="O12" t="n">
+        <v>-548.7929538670101</v>
+      </c>
+      <c r="P12" t="n">
+        <v>-548.7929538670101</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>-513.0088329597651</v>
+      </c>
+      <c r="R12" t="n">
+        <v>-453.6275175247511</v>
+      </c>
+      <c r="S12" t="n">
+        <v>-453.6275175247511</v>
+      </c>
+      <c r="T12" t="n">
+        <v>-453.6275175247511</v>
+      </c>
+      <c r="U12" t="n">
+        <v>-490.27208051843</v>
+      </c>
+      <c r="V12" t="n">
+        <v>-490.27208051843</v>
+      </c>
+      <c r="W12" t="n">
+        <v>-490.27208051843</v>
+      </c>
+      <c r="X12" t="n">
+        <v>-490.27208051843</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>-490.27208051843</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>-465.3125497698164</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>-453</v>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>sub(x3, ang_vel(tan(x3), asin(x1, limit(add(acos(add(y3, x1), add(add(y2, y3), tan(y1))), y3), acos(y3, x3), asin(y1, x2))), max(tan(protectedDiv(x1, y1)), acos(x1, y2)), x1))</t>
+        </is>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">atan, conditional, cos, sin, </t>
+        </is>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">max, tan, ang_vel, y2, sub, limit, y1, protectedDiv, acos, x2, x1, y3, x3, add, asin, </t>
+        </is>
+      </c>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>replace</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>